<commit_message>
[ADD] field offset_footer in mapping
</commit_message>
<xml_diff>
--- a/account_statement_import_txt_xlsx/tests/fixtures/sample_statement_offsets.xlsx
+++ b/account_statement_import_txt_xlsx/tests/fixtures/sample_statement_offsets.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">Azure Interior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any footer data</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -157,6 +160,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -171,132 +178,26 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -385,6 +286,22 @@
       </c>
       <c r="H5" s="2"/>
     </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>